<commit_message>
Updated Planned Stats and Layout
An ongoing update to flesh out random drops.
</commit_message>
<xml_diff>
--- a/Castle Fayyt - Planned Stats.xlsx
+++ b/Castle Fayyt - Planned Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\Castle-Fayyt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22160C6F-6FAF-48FB-982E-4B297D9B946E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED932322-918E-41A5-884B-36209EE2EE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="5" xr2:uid="{E5B59356-4BF5-46FB-97E4-B22FBEC1131D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{E5B59356-4BF5-46FB-97E4-B22FBEC1131D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
   <si>
     <t>fight</t>
   </si>
@@ -290,9 +290,6 @@
     <t>Coin</t>
   </si>
   <si>
-    <t>key (small treasure)</t>
-  </si>
-  <si>
     <t>crow brooch</t>
   </si>
   <si>
@@ -308,24 +305,9 @@
     <t>amethyst</t>
   </si>
   <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
     <t>diamond</t>
   </si>
   <si>
-    <t>yellow</t>
-  </si>
-  <si>
     <t>tiny treasure box</t>
   </si>
   <si>
@@ -339,9 +321,6 @@
   </si>
   <si>
     <t>Watch Fob</t>
-  </si>
-  <si>
-    <t>Bejeweled with Bloodstones</t>
   </si>
   <si>
     <t>d-20</t>
@@ -466,6 +445,108 @@
     </r>
   </si>
   <si>
+    <t>Malfunctioning Jock Strap</t>
+  </si>
+  <si>
+    <t>Artensian Spell Book</t>
+  </si>
+  <si>
+    <t>Fight only</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Magic only</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Text to be displayed on calling Inventory</t>
+  </si>
+  <si>
+    <t>Set Details</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Random drop from a monster (outside of mandatory path.)</t>
+  </si>
+  <si>
+    <t>Automatically given to player when they have both.</t>
+  </si>
+  <si>
+    <t>a tiny key</t>
+  </si>
+  <si>
+    <t>This tiny key looks like it will fit a very tiny lock.  Definitely part of a child's treasured memory.</t>
+  </si>
+  <si>
+    <t>This tiny treasure box looks like something a child would, well, treasure.  It is ornately decorated with crayon scrawled hearts and tiny stick figures in postures of play with larger stick figures… like a family.</t>
+  </si>
+  <si>
+    <t>A brilliant green gem set in a brass clasp with a hook on one side, and a complimentary ring on the other, as if it were meant to attach to a set of gems...</t>
+  </si>
+  <si>
+    <t>A blood-red gem set in a silver clasp with a hook on one side, and a complimentary ring on the other, as if it were meant to attach to a set of gems...</t>
+  </si>
+  <si>
+    <t>A stunningly yellow gem set in a gold clasp with a hook on one side, and a complimentary ring on the other, as if it were meant to attach to a set of gems...</t>
+  </si>
+  <si>
+    <t>A shimmering blue gem set in a lead clasp with a hook on one side, and a complimentary ring on the other, as if it were meant to attach to a set of gems...</t>
+  </si>
+  <si>
+    <t>A deep purple gem set in a copper clasp with a hook on one side, and a complimentary ring on the other, as if it were meant to attach to a set of gems...</t>
+  </si>
+  <si>
+    <t>Rainbow Gem Set</t>
+  </si>
+  <si>
+    <t>The five gems-- emerald, ruby, diamond, sapphire, and amethyst-- lock together to form a tight circlet that perfectly fits your wrist as a bracelet.  (Adds 2 points of magic damage against standard enemies.)</t>
+  </si>
+  <si>
+    <t>Created when player has all five of the gems.</t>
+  </si>
+  <si>
+    <t>Only available from monster drops.</t>
+  </si>
+  <si>
+    <t>Random drop in rooms</t>
+  </si>
+  <si>
+    <t>A Certain Sartorial Elegance</t>
+  </si>
+  <si>
+    <t>And a style that's almost all your own.  (Causes five points of damage every time you enter a room.  Impossible to remove.)</t>
+  </si>
+  <si>
+    <t>Created when player has all four of the Sartorial Elegance set items.</t>
+  </si>
+  <si>
+    <t>This absolutely gorgeous silver brooch with obsidian flecks exquisitely matches your dark leather jerkin.  The chips of garnet set in the eyes seem to bathe every corner of the room with a faint reddish glow.</t>
+  </si>
+  <si>
+    <t>This jade pin set in a lead backing is so finely detailed that the tiny green point of the arrow shimmers as if liquescent.  Fits perfectly on your headgear.</t>
+  </si>
+  <si>
+    <t>This silver locket has been cast with a pouncing panther on its front, claws clearly rising from the lower right as if to rip apart its intended prey.  The back features the paw prints depressed into the metal.  Whenever you open the locket, it smells slightly of almonds.</t>
+  </si>
+  <si>
+    <t>This gold watch fob is just the thing for keeping time.  The magic that moves the hands around the circular dial are still working, even after all these millenia.  And the bloodstone insets are simply breathtaking.</t>
+  </si>
+  <si>
+    <t>Jumanji starter kit dice set</t>
+  </si>
+  <si>
+    <t>This  dodecahedron features a smoky green color, shot through with flecks of brown and white.  You're fairly certain it's a green agate.  It seems to roll well, and the numbers on each face have a truly random probability spread.</t>
+  </si>
+  <si>
+    <t>This looks like a tooth that a six-year-old child might lose.  Due to the fact that it hasn't decayed through the centuries, you are certain this is Fayyt Ignatti's baby tooth.  It might still have sentimental value to her.  (Gives a -5 to damage for each of Fayyt's attacks.)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -486,34 +567,55 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Give a -1 attack to Fayyt
+Give a -5 attack to Fayyt
 </t>
     </r>
   </si>
   <si>
-    <t>Malfunctioning Jock Strap</t>
-  </si>
-  <si>
-    <t>Artensian Spell Book</t>
-  </si>
-  <si>
-    <t>Fight only</t>
-  </si>
-  <si>
-    <t>Attack</t>
-  </si>
-  <si>
-    <t>Magic only</t>
-  </si>
-  <si>
-    <t>Random</t>
+    <t>This opaque yellow icosohedron seems to be made from amber.  It has unique, black numbers etched on each face ranging from one to twenty.  You can tell from experience that this is not a loaded die.  It rolls true.</t>
+  </si>
+  <si>
+    <t>You are certain that this decaherdon is made of bone.  What you aren't certain of is the origin of the bone.  Is it human, animal, or monstrosity?  The numbers on the faces are painted a deep red, in a morbid attempt to suggest blood.</t>
+  </si>
+  <si>
+    <t>The octohedron made of cheap, translucent plastic is perfectly ordinary.  You have about thirty of these back in your home, and get together with your party every third Wednesday of the month.  The Paladin in your group is such a bard…</t>
+  </si>
+  <si>
+    <t>The corners and edges of this blown-glass hexahedron were thankfully softened to curves.  You dare not try rolling this one, for fear of breaking such a delicate treasure.  The numbers on the six faces are hand painted in blue.</t>
+  </si>
+  <si>
+    <t>Tetrahedron.  This is a tetrahedron.  Four sides.  Black.  Heavy as a 30 pound bag of…. anything that's 30 pounds. So small that it fits in exactly the same amount of space as a four-sided die.  Which it is.  It's a tetrahedron.</t>
+  </si>
+  <si>
+    <t>This remarkably mismatched dice set always seems to roll natural twenties when enemies attack.  (Increases the chances that a monster will roll critical hit damage.  Impossible to drop.)</t>
+  </si>
+  <si>
+    <t>Created when player has all six of the game dice.</t>
+  </si>
+  <si>
+    <t>Soiled handkerchief</t>
+  </si>
+  <si>
+    <t>Been used as many times as inventory is called.</t>
+  </si>
+  <si>
+    <t>Taxidermied rat</t>
+  </si>
+  <si>
+    <t>Crystal skull</t>
+  </si>
+  <si>
+    <t>Blockbuster Video membership card</t>
+  </si>
+  <si>
+    <t>Toupee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,8 +637,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,8 +700,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -615,11 +742,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,39 +823,107 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,6 +932,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FF99"/>
       <color rgb="FFCC99FF"/>
     </mruColors>
   </colors>
@@ -1406,857 +1652,1500 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6364C51-5053-4748-A0B4-E506C4620EAD}">
-  <dimension ref="C4:S36"/>
+  <dimension ref="C4:AA44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:E22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27:S27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="26" max="27" width="9.140625" style="43"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="28" t="s">
+    <row r="4" spans="3:27" ht="21.95" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-    </row>
-    <row r="5" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="12">
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+    </row>
+    <row r="5" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28">
         <v>1</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-    </row>
-    <row r="6" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="G5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="40"/>
+      <c r="Z5" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12">
         <v>2</v>
       </c>
-      <c r="G6" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-    </row>
-    <row r="7" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="G6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="AA6" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12">
         <v>3</v>
       </c>
-      <c r="G7" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-    </row>
-    <row r="8" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="G7" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="42"/>
+    </row>
+    <row r="8" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C8" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12">
         <v>4</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
-      <c r="K8" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-    </row>
-    <row r="9" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="K8" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="40"/>
+      <c r="Z8" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12">
         <v>5</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
-      <c r="K9" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-    </row>
-    <row r="10" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="K9" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="AA9" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12">
         <v>6</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
-      <c r="K10" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-    </row>
-    <row r="11" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="K10" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="40"/>
+      <c r="Z10" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12">
         <v>7</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
-      <c r="K11" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-    </row>
-    <row r="12" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="12">
+      <c r="K11" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="39"/>
+      <c r="Y11" s="40"/>
+      <c r="Z11" s="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="16">
         <v>8</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-    </row>
-    <row r="13" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="K12" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12">
         <v>9</v>
       </c>
-      <c r="G13" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-    </row>
-    <row r="14" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="19"/>
+      <c r="G13" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+    </row>
+    <row r="14" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="19" t="s">
+        <v>114</v>
+      </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="12">
         <v>10</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-    </row>
-    <row r="15" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="40"/>
+      <c r="Z14" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="12">
+      <c r="F15" s="16">
         <v>11</v>
       </c>
-      <c r="G15" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-    </row>
-    <row r="16" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="U15" s="39"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="39"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="12">
+      <c r="F16" s="16">
         <v>12</v>
       </c>
-      <c r="G16" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-    </row>
-    <row r="17" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
-        <v>119</v>
-      </c>
+      <c r="G16" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="AA16" s="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
-      <c r="F17" s="12">
+      <c r="F17" s="16">
         <v>13</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-    </row>
-    <row r="18" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="40"/>
+      <c r="Z17" s="43">
+        <v>7</v>
+      </c>
+      <c r="AA17" s="43"/>
+    </row>
+    <row r="18" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="12">
+      <c r="F18" s="16">
         <v>14</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-    </row>
-    <row r="19" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="19"/>
+      <c r="G18" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+    </row>
+    <row r="19" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C19" s="19" t="s">
+        <v>112</v>
+      </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="12">
+      <c r="F19" s="16">
         <v>15</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-    </row>
-    <row r="20" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41"/>
+      <c r="AA19" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
-      <c r="F20" s="12">
+      <c r="F20" s="16">
         <v>16</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-    </row>
-    <row r="21" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="12">
+      <c r="F21" s="16">
         <v>17</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-    </row>
-    <row r="22" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
+      <c r="AA21" s="43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="12">
+      <c r="F22" s="16">
         <v>18</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-    </row>
-    <row r="23" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12">
+      <c r="G22" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U22" s="39"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="39"/>
+      <c r="X22" s="39"/>
+      <c r="Y22" s="40"/>
+      <c r="Z22" s="43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="16">
         <v>19</v>
       </c>
-      <c r="G23" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-    </row>
-    <row r="24" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12">
+      <c r="G23" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="39"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U24" s="39"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="39"/>
+      <c r="X24" s="39"/>
+      <c r="Y24" s="40"/>
+      <c r="Z24" s="43">
+        <v>11</v>
+      </c>
+      <c r="AA24" s="43"/>
+    </row>
+    <row r="25" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="16">
         <v>20</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-    </row>
-    <row r="25" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12">
-        <v>21</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-    </row>
-    <row r="26" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="U25" s="42"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="42"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+    </row>
+    <row r="26" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="12">
-        <v>22</v>
+      <c r="F26" s="16">
+        <v>21</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-    </row>
-    <row r="27" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U26" s="39"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+      <c r="Y26" s="40"/>
+      <c r="Z26" s="43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="12">
-        <v>23</v>
+      <c r="F27" s="16">
+        <v>22</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-    </row>
-    <row r="28" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U27" s="41"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="AA27" s="43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="12">
-        <v>24</v>
+      <c r="F28" s="16">
+        <v>23</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-    </row>
-    <row r="29" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U28" s="39"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="40"/>
+      <c r="Z28" s="43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="12">
-        <v>25</v>
+      <c r="F29" s="16">
+        <v>24</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
-    </row>
-    <row r="30" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U29" s="39"/>
+      <c r="V29" s="39"/>
+      <c r="W29" s="39"/>
+      <c r="X29" s="39"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="43">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="12">
-        <v>26</v>
+      <c r="F30" s="16">
+        <v>25</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-    </row>
-    <row r="31" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="37"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U30" s="39"/>
+      <c r="V30" s="39"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="40"/>
+      <c r="Z30" s="43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
-      <c r="F31" s="12">
-        <v>27</v>
+      <c r="F31" s="16">
+        <v>26</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
-      <c r="K31" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-    </row>
-    <row r="32" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U31" s="41"/>
+      <c r="V31" s="41"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="AA31" s="43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="12">
-        <v>28</v>
+      <c r="F32" s="16">
+        <v>27</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
       <c r="J32" s="17"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-    </row>
-    <row r="33" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U32" s="41"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="41"/>
+      <c r="AA32" s="43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="12">
-        <v>29</v>
+      <c r="F33" s="16">
+        <v>28</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
       <c r="J33" s="17"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-    </row>
-    <row r="34" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="37"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="37"/>
+      <c r="T33" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U33" s="39"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="12">
-        <v>30</v>
+      <c r="F34" s="16">
+        <v>29</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-    </row>
-    <row r="35" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="37"/>
+      <c r="R34" s="37"/>
+      <c r="S34" s="37"/>
+      <c r="T34" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="43">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="12">
-        <v>31</v>
+      <c r="F35" s="16">
+        <v>30</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-    </row>
-    <row r="36" spans="3:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
+      <c r="S35" s="37"/>
+      <c r="T35" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U35" s="39"/>
+      <c r="V35" s="39"/>
+      <c r="W35" s="39"/>
+      <c r="X35" s="39"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="43">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
-      <c r="F36" s="12">
-        <v>32</v>
+      <c r="F36" s="16">
+        <v>31</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H36" s="17"/>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="37"/>
+      <c r="S36" s="37"/>
+      <c r="T36" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="41"/>
+      <c r="AA36" s="43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="16">
+        <v>32</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U37" s="39"/>
+      <c r="V37" s="39"/>
+      <c r="W37" s="39"/>
+      <c r="X37" s="39"/>
+      <c r="Y37" s="40"/>
+      <c r="Z37" s="43">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="16">
+        <v>33</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="41"/>
+      <c r="X38" s="41"/>
+      <c r="Y38" s="41"/>
+      <c r="AA38" s="43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="16">
+        <v>34</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U39" s="39"/>
+      <c r="V39" s="39"/>
+      <c r="W39" s="39"/>
+      <c r="X39" s="39"/>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="3:27" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F40" s="16">
+        <v>35</v>
+      </c>
+      <c r="G40" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="46"/>
+      <c r="T40" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="U40" s="51"/>
+      <c r="V40" s="51"/>
+      <c r="W40" s="51"/>
+      <c r="X40" s="51"/>
+      <c r="Y40" s="52"/>
+      <c r="AA40" s="43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="3:27" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F41" s="16">
+        <v>36</v>
+      </c>
+      <c r="G41" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
+      <c r="O41" s="45"/>
+      <c r="P41" s="45"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
+      <c r="S41" s="46"/>
+      <c r="T41" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U41" s="39"/>
+      <c r="V41" s="39"/>
+      <c r="W41" s="39"/>
+      <c r="X41" s="39"/>
+      <c r="Y41" s="40"/>
+      <c r="Z41" s="43">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="3:27" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F42" s="16">
+        <v>37</v>
+      </c>
+      <c r="G42" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="45"/>
+      <c r="N42" s="45"/>
+      <c r="O42" s="45"/>
+      <c r="P42" s="45"/>
+      <c r="Q42" s="45"/>
+      <c r="R42" s="45"/>
+      <c r="S42" s="46"/>
+      <c r="T42" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="U42" s="39"/>
+      <c r="V42" s="39"/>
+      <c r="W42" s="39"/>
+      <c r="X42" s="39"/>
+      <c r="Y42" s="40"/>
+      <c r="Z42" s="43">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="3:27" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F43" s="16">
+        <v>38</v>
+      </c>
+      <c r="G43" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="45"/>
+      <c r="M43" s="45"/>
+      <c r="N43" s="45"/>
+      <c r="O43" s="45"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="46"/>
+      <c r="T43" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="U43" s="51"/>
+      <c r="V43" s="51"/>
+      <c r="W43" s="51"/>
+      <c r="X43" s="51"/>
+      <c r="Y43" s="52"/>
+      <c r="AA43" s="43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="3:27" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F44" s="16">
+        <v>39</v>
+      </c>
+      <c r="G44" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="45"/>
+      <c r="M44" s="45"/>
+      <c r="N44" s="45"/>
+      <c r="O44" s="45"/>
+      <c r="P44" s="45"/>
+      <c r="Q44" s="45"/>
+      <c r="R44" s="45"/>
+      <c r="S44" s="46"/>
+      <c r="T44" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="U44" s="51"/>
+      <c r="V44" s="51"/>
+      <c r="W44" s="51"/>
+      <c r="X44" s="51"/>
+      <c r="Y44" s="52"/>
+      <c r="AA44" s="43">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="69">
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="K34:S34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="K35:S35"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="K36:S36"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="K31:S31"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:S32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="K33:S33"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="K28:S28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:S29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="K30:S30"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="K25:S25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="K26:S26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="K27:S27"/>
-    <mergeCell ref="K21:S21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="K22:S22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="K23:S23"/>
+  <mergeCells count="128">
+    <mergeCell ref="T43:Y43"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="K44:S44"/>
+    <mergeCell ref="T44:Y44"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K42:S42"/>
+    <mergeCell ref="T42:Y42"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="K43:S43"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:S40"/>
+    <mergeCell ref="T40:Y40"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="K41:S41"/>
+    <mergeCell ref="T41:Y41"/>
+    <mergeCell ref="T39:Y39"/>
+    <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="K12:S12"/>
+    <mergeCell ref="T12:Y12"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:S17"/>
+    <mergeCell ref="T17:Y17"/>
     <mergeCell ref="G24:J24"/>
     <mergeCell ref="K24:S24"/>
-    <mergeCell ref="C17:E22"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:S17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="K18:S18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="K19:S19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="K20:S20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K12:S12"/>
-    <mergeCell ref="C13:E16"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:S13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:S14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="K15:S15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="K16:S16"/>
-    <mergeCell ref="C8:E12"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K8:S8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="K9:S9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:S10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:S11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="T24:Y24"/>
+    <mergeCell ref="T5:Y5"/>
+    <mergeCell ref="T6:Y6"/>
+    <mergeCell ref="T7:Y7"/>
+    <mergeCell ref="T8:Y8"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="T11:Y11"/>
+    <mergeCell ref="T13:Y13"/>
+    <mergeCell ref="T14:Y14"/>
+    <mergeCell ref="T15:Y15"/>
+    <mergeCell ref="T16:Y16"/>
+    <mergeCell ref="T18:Y18"/>
+    <mergeCell ref="T19:Y19"/>
+    <mergeCell ref="T20:Y20"/>
+    <mergeCell ref="T21:Y21"/>
+    <mergeCell ref="T34:Y34"/>
+    <mergeCell ref="T35:Y35"/>
+    <mergeCell ref="T36:Y36"/>
+    <mergeCell ref="T37:Y37"/>
+    <mergeCell ref="T38:Y38"/>
+    <mergeCell ref="T29:Y29"/>
+    <mergeCell ref="T30:Y30"/>
+    <mergeCell ref="T31:Y31"/>
+    <mergeCell ref="T32:Y32"/>
+    <mergeCell ref="T33:Y33"/>
+    <mergeCell ref="T23:Y23"/>
+    <mergeCell ref="T25:Y25"/>
+    <mergeCell ref="T26:Y26"/>
+    <mergeCell ref="T27:Y27"/>
+    <mergeCell ref="T28:Y28"/>
+    <mergeCell ref="T22:Y22"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:S4"/>
     <mergeCell ref="C5:E7"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="K5:S5"/>
@@ -2264,8 +3153,70 @@
     <mergeCell ref="K6:S6"/>
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="K7:S7"/>
+    <mergeCell ref="K10:S10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:S11"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:S13"/>
+    <mergeCell ref="C14:E18"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:S14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:S15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:S16"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:S18"/>
+    <mergeCell ref="C8:E13"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:S8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="K9:S9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:S27"/>
+    <mergeCell ref="C19:E25"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K20:S20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:S21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="K22:S22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="K23:S23"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="K25:S25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="K26:S26"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:S28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:S29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="K30:S30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="K31:S31"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:S32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="K33:S33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="K34:S34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="K35:S35"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="K36:S36"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:S37"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="K38:S38"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="K39:S39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3514,7 +4465,7 @@
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
@@ -3918,7 +4869,7 @@
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -4214,7 +5165,7 @@
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
       <c r="X28" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="Y28" s="11"/>
       <c r="Z28" s="11"/>
@@ -5098,7 +6049,7 @@
       <c r="V38" s="11"/>
       <c r="W38" s="11"/>
       <c r="X38" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="Y38" s="11"/>
       <c r="Z38" s="11"/>
@@ -5704,11 +6655,11 @@
       <c r="F49" s="10">
         <v>1</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
@@ -5758,11 +6709,11 @@
       <c r="F50" s="10">
         <v>2</v>
       </c>
-      <c r="G50" s="29" t="s">
+      <c r="G50" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11" t="s">
         <v>54</v>
@@ -5814,11 +6765,11 @@
       <c r="F51" s="10">
         <v>3</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11" t="s">
         <v>55</v>
@@ -5870,11 +6821,11 @@
       <c r="F52" s="10">
         <v>4</v>
       </c>
-      <c r="G52" s="29" t="s">
+      <c r="G52" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11" t="s">
         <v>56</v>
@@ -5926,11 +6877,11 @@
       <c r="F53" s="10">
         <v>5</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="G53" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
@@ -5980,11 +6931,11 @@
       <c r="F54" s="10">
         <v>6</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G54" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
       <c r="L54" s="11"/>
@@ -6034,11 +6985,11 @@
       <c r="F55" s="10">
         <v>7</v>
       </c>
-      <c r="G55" s="29" t="s">
+      <c r="G55" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
       <c r="L55" s="11"/>
@@ -6082,11 +7033,11 @@
       <c r="F56" s="10">
         <v>8</v>
       </c>
-      <c r="G56" s="29" t="s">
+      <c r="G56" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H56" s="29"/>
-      <c r="I56" s="29"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
       <c r="L56" s="11"/>
@@ -6130,11 +7081,11 @@
       <c r="F57" s="10">
         <v>9</v>
       </c>
-      <c r="G57" s="29" t="s">
+      <c r="G57" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="H57" s="29"/>
-      <c r="I57" s="29"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
@@ -6178,11 +7129,11 @@
       <c r="F58" s="10">
         <v>10</v>
       </c>
-      <c r="G58" s="29" t="s">
+      <c r="G58" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
       <c r="L58" s="11"/>
@@ -6870,7 +7821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4739A14-FE6D-41AD-978E-AB615AC2B33D}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
@@ -6911,15 +7862,15 @@
       <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="15" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="11">
         <v>1</v>
       </c>
@@ -6929,15 +7880,15 @@
       <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="15" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="11">
         <v>2</v>
       </c>
@@ -6947,15 +7898,15 @@
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="11">
         <v>3</v>
       </c>
@@ -6965,15 +7916,15 @@
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="15" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="11">
         <v>3</v>
       </c>
@@ -6983,15 +7934,15 @@
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="15" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="11">
         <v>4</v>
       </c>
@@ -7001,15 +7952,15 @@
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="15" t="s">
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="11">
         <v>5</v>
       </c>
@@ -7019,15 +7970,15 @@
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="11">
         <v>6</v>
       </c>
@@ -7037,15 +7988,15 @@
       <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="15" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="11">
         <v>4</v>
       </c>
@@ -7055,15 +8006,15 @@
       <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="15" t="s">
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="11">
         <v>5</v>
       </c>
@@ -7073,15 +8024,15 @@
       <c r="B13" s="9">
         <v>10</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="15" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="11">
         <v>3</v>
       </c>
@@ -7091,15 +8042,15 @@
       <c r="B14" s="9">
         <v>11</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="15" t="s">
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="11">
         <v>5</v>
       </c>
@@ -7109,38 +8060,38 @@
       <c r="B15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Castle Fayyt - Planned Stats.xlsx
Finished writing out the planned random drops and flavor text to show when called from inventory.
</commit_message>
<xml_diff>
--- a/Castle Fayyt - Planned Stats.xlsx
+++ b/Castle Fayyt - Planned Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\Castle-Fayyt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED932322-918E-41A5-884B-36209EE2EE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E485105A-3E96-4B38-8A57-E97C29D3EF4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{E5B59356-4BF5-46FB-97E4-B22FBEC1131D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="180">
   <si>
     <t>fight</t>
   </si>
@@ -360,9 +360,6 @@
   </si>
   <si>
     <t>Ball of twine</t>
-  </si>
-  <si>
-    <t>Grows 2 inches shorter each time you call inventory until it disappears.</t>
   </si>
   <si>
     <t>Dragon-fang necklace</t>
@@ -596,9 +593,6 @@
     <t>Soiled handkerchief</t>
   </si>
   <si>
-    <t>Been used as many times as inventory is called.</t>
-  </si>
-  <si>
     <t>Taxidermied rat</t>
   </si>
   <si>
@@ -609,6 +603,63 @@
   </si>
   <si>
     <t>Toupee</t>
+  </si>
+  <si>
+    <t>It's shiny.  It's a rock.  It's not a gem, or a precious metal.  But it's really shiny.  And it's a rock.</t>
+  </si>
+  <si>
+    <t>This heavy, silver candlestick has been cast in the shape of a dancing Sarthinian girl.  The flowing scarves around her neck and wrists wrapping upward to hold the candles.  Although it could technically be used as a bludgeoning weapon, it would make a better keepsake.</t>
+  </si>
+  <si>
+    <t>This commemorative silver dallir in a cryoforged plastic vision sleeve is the perfect gift for all the loved ones in your life.  Not only does the decorative front feature the victorious Nimbilts returning from battle with the Artensians, but the back is finely etched with the grand surrender of the Artensians as photorendered by military journalist, Pierce Rhyley.</t>
+  </si>
+  <si>
+    <t>Something about this dagger suggests that it might be older than Castle Fayyt itself.  Older than the historical record.  Something known only from the oral traditions as a place called shong kwa.</t>
+  </si>
+  <si>
+    <t>A very simple iron kettle.  It has a few dents.  Black scorch marks on the base show that it was well-used.  You'd probably still be able to use it to boil liquids if you wanted to.</t>
+  </si>
+  <si>
+    <t>Shimmering liquid sloshes about in this vial even when you don't move it.  It makes your pocket feel funny.  You briefly wonder what made the fairies cry.</t>
+  </si>
+  <si>
+    <t>A black bag with a drawstring holds toenail clippings of all sizes and in differing degrees of cleanliness.  There are big yellow ones, small white ones.  A couple covered in a dark red substance.  Just don't mistake this bag for your trail rations.</t>
+  </si>
+  <si>
+    <t>This chastity belt fulfilled its purpose.  You can see where there are faint scratches on the bolts that hold it together.  Although your enlightened age would never use such a cruel and heinous object, the key is in the lock, so chances are you could force it on another unwilling victim-- er.. woman... For her protection, of course.</t>
+  </si>
+  <si>
+    <t>A [random color] ball of twine about 120 inches in length.  (Grows 2 inches shorter each time you call inventory until it disappears.)</t>
+  </si>
+  <si>
+    <t>The sheer number of dragons that gave their dental consent to make this necklace is staggering.  At least one!!  I mean, who would go talk to a dragon to ask it for teeth.  It's like belling a cat.</t>
+  </si>
+  <si>
+    <t>This small statue of an elephant glows with its own native light source.  You can't detect any magical energies coming from it.  Looks like it was just formed from a naturally glowing material.</t>
+  </si>
+  <si>
+    <t>Even if you can't see it, you know it's there.</t>
+  </si>
+  <si>
+    <t>The cracks and snapped lines of this jockstrap have been hastily covered with superglue and duct tape.  All to no avail.  It won't protect anybodie's family jewels ever again.</t>
+  </si>
+  <si>
+    <t>When the Artensians dared to settle on the spit of land between the Syryth Ocean and the Blue Sea, they unwittingly began their own mass destruction.  Their mages fought tirelessly against the brave Nimbiltish warriors.  In the end, though, their hubris and lack of magical prowess doomed them to failure.  This Spell Book, written in Artensian, would make great kindling for a fire now.</t>
+  </si>
+  <si>
+    <t>Covered in dry white and green spots, this handkerchief has been use about [as many times as inventory has been called; counting begins at game start, not when item is found] times.</t>
+  </si>
+  <si>
+    <t>Small creature that looks something like a Hari Cat, but much, much smaller.  The ears are a little rounder, and the tail is smaller and straighter.  The stuffed creature looks like it could easily still bite you with its sharp yellow fangs.</t>
+  </si>
+  <si>
+    <t>From a kingdom lost to antiquity.  Also from a workshop lost to antiquity.  Some people say these things have paranormal powers.  You haven't observed any truth to that claim.</t>
+  </si>
+  <si>
+    <t>Blue and white with yellow lettering, this distinctive card is lovingly wrapped in cellophane and heat-dried to resist water damage.  You'll be able to observe videomimeographines for days to come with this bad boy.</t>
+  </si>
+  <si>
+    <t>Why is it that whenever you wear this yellow, very obvious fake hair piece, the wind starts to blow?  And your skin turns a little bit orange.  Must have very potent powers indeed!  Unfortunately, that's the extent of the powers you've been able to deduce.</t>
   </si>
 </sst>
 </file>
@@ -824,61 +875,57 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -896,7 +943,15 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -905,15 +960,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -924,6 +970,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1654,22 +1705,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6364C51-5053-4748-A0B4-E506C4620EAD}">
   <dimension ref="C4:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27:S27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="26" max="27" width="9.140625" style="43"/>
+    <col min="26" max="27" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:27" ht="21.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C4" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="30" t="s">
         <v>81</v>
       </c>
@@ -1677,7 +1728,7 @@
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
       <c r="K4" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
@@ -1688,7 +1739,7 @@
       <c r="R4" s="30"/>
       <c r="S4" s="30"/>
       <c r="T4" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U4" s="30"/>
       <c r="V4" s="30"/>
@@ -1697,757 +1748,757 @@
       <c r="Y4" s="30"/>
     </row>
     <row r="5" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28">
+      <c r="C5" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="17">
         <v>1</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="43">
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="12">
         <v>2</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="AA6" s="43">
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="AA6" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="12">
         <v>3</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="40"/>
     </row>
     <row r="8" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C8" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="C8" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="12">
         <v>4</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="40"/>
-      <c r="Z8" s="43">
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="12">
         <v>5</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="AA9" s="43">
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="39"/>
+      <c r="AA9" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="12">
         <v>6</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="43">
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
       <c r="F11" s="12">
         <v>7</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="39"/>
-      <c r="X11" s="39"/>
-      <c r="Y11" s="40"/>
-      <c r="Z11" s="43">
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="16">
         <v>8</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43">
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="12">
         <v>9</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="34" t="s">
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="U13" s="42"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
-      <c r="X13" s="42"/>
-      <c r="Y13" s="42"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
     </row>
     <row r="14" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="C14" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="12">
         <v>10</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
-      <c r="X14" s="39"/>
-      <c r="Y14" s="40"/>
-      <c r="Z14" s="43">
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="16">
         <v>11</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="U15" s="39"/>
-      <c r="V15" s="39"/>
-      <c r="W15" s="39"/>
-      <c r="X15" s="39"/>
-      <c r="Y15" s="40"/>
-      <c r="Z15" s="43">
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="38"/>
+      <c r="Z15" s="19">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="16">
         <v>12</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U16" s="41"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="41"/>
-      <c r="AA16" s="43">
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="AA16" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="16">
         <v>13</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="39"/>
-      <c r="X17" s="39"/>
-      <c r="Y17" s="40"/>
-      <c r="Z17" s="43">
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="19">
         <v>7</v>
       </c>
-      <c r="AA17" s="43"/>
+      <c r="AA17" s="19"/>
     </row>
     <row r="18" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="16">
         <v>14</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="35" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="U18" s="42"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="42"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
     </row>
     <row r="19" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C19" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="C19" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="16">
         <v>15</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="41"/>
-      <c r="AA19" s="43">
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+      <c r="Y19" s="39"/>
+      <c r="AA19" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="16">
         <v>16</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39"/>
-      <c r="W20" s="39"/>
-      <c r="X20" s="39"/>
-      <c r="Y20" s="40"/>
-      <c r="Z20" s="43">
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="37"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="19">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="16">
         <v>17</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U21" s="41"/>
-      <c r="V21" s="41"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="41"/>
-      <c r="Y21" s="41"/>
-      <c r="AA21" s="43">
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="39"/>
+      <c r="AA21" s="19">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="16">
         <v>18</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U22" s="39"/>
-      <c r="V22" s="39"/>
-      <c r="W22" s="39"/>
-      <c r="X22" s="39"/>
-      <c r="Y22" s="40"/>
-      <c r="Z22" s="43">
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="38"/>
+      <c r="Z22" s="19">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="16">
         <v>19</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="36" t="s">
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U23" s="39"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
-      <c r="X23" s="39"/>
-      <c r="Y23" s="40"/>
-      <c r="Z23" s="43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="3:27" s="15" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U24" s="39"/>
-      <c r="V24" s="39"/>
-      <c r="W24" s="39"/>
-      <c r="X24" s="39"/>
-      <c r="Y24" s="40"/>
-      <c r="Z24" s="43">
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="38"/>
+      <c r="Z24" s="19">
         <v>11</v>
       </c>
-      <c r="AA24" s="43"/>
+      <c r="AA24" s="19"/>
     </row>
     <row r="25" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="16">
         <v>20</v>
       </c>
-      <c r="G25" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="36" t="s">
+      <c r="G25" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="U25" s="42"/>
-      <c r="V25" s="42"/>
-      <c r="W25" s="42"/>
-      <c r="X25" s="42"/>
-      <c r="Y25" s="42"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="40"/>
+      <c r="X25" s="40"/>
+      <c r="Y25" s="40"/>
     </row>
     <row r="26" spans="3:27" ht="48" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C26" s="11"/>
@@ -2456,30 +2507,32 @@
       <c r="F26" s="16">
         <v>21</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="37"/>
-      <c r="R26" s="37"/>
-      <c r="S26" s="37"/>
-      <c r="T26" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U26" s="39"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="39"/>
-      <c r="X26" s="39"/>
-      <c r="Y26" s="40"/>
-      <c r="Z26" s="43">
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="37"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="19">
         <v>12</v>
       </c>
     </row>
@@ -2490,30 +2543,32 @@
       <c r="F27" s="16">
         <v>22</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U27" s="41"/>
-      <c r="V27" s="41"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41"/>
-      <c r="AA27" s="43">
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U27" s="39"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="39"/>
+      <c r="Y27" s="39"/>
+      <c r="AA27" s="19">
         <v>7</v>
       </c>
     </row>
@@ -2524,30 +2579,32 @@
       <c r="F28" s="16">
         <v>23</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U28" s="39"/>
-      <c r="V28" s="39"/>
-      <c r="W28" s="39"/>
-      <c r="X28" s="39"/>
-      <c r="Y28" s="40"/>
-      <c r="Z28" s="43">
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
+      <c r="W28" s="37"/>
+      <c r="X28" s="37"/>
+      <c r="Y28" s="38"/>
+      <c r="Z28" s="19">
         <v>13</v>
       </c>
     </row>
@@ -2558,30 +2615,32 @@
       <c r="F29" s="16">
         <v>24</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="40"/>
-      <c r="Z29" s="43">
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="38"/>
+      <c r="Z29" s="19">
         <v>14</v>
       </c>
     </row>
@@ -2592,30 +2651,32 @@
       <c r="F30" s="16">
         <v>25</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="37"/>
-      <c r="Q30" s="37"/>
-      <c r="R30" s="37"/>
-      <c r="S30" s="37"/>
-      <c r="T30" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U30" s="39"/>
-      <c r="V30" s="39"/>
-      <c r="W30" s="39"/>
-      <c r="X30" s="39"/>
-      <c r="Y30" s="40"/>
-      <c r="Z30" s="43">
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U30" s="37"/>
+      <c r="V30" s="37"/>
+      <c r="W30" s="37"/>
+      <c r="X30" s="37"/>
+      <c r="Y30" s="38"/>
+      <c r="Z30" s="19">
         <v>15</v>
       </c>
     </row>
@@ -2626,30 +2687,32 @@
       <c r="F31" s="16">
         <v>26</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="37"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U31" s="41"/>
-      <c r="V31" s="41"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="41"/>
-      <c r="Y31" s="41"/>
-      <c r="AA31" s="43">
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="AA31" s="19">
         <v>8</v>
       </c>
     </row>
@@ -2660,30 +2723,32 @@
       <c r="F32" s="16">
         <v>27</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U32" s="41"/>
-      <c r="V32" s="41"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="41"/>
-      <c r="Y32" s="41"/>
-      <c r="AA32" s="43">
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="AA32" s="19">
         <v>9</v>
       </c>
     </row>
@@ -2694,30 +2759,32 @@
       <c r="F33" s="16">
         <v>28</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U33" s="39"/>
-      <c r="V33" s="39"/>
-      <c r="W33" s="39"/>
-      <c r="X33" s="39"/>
-      <c r="Y33" s="40"/>
-      <c r="Z33" s="43">
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U33" s="37"/>
+      <c r="V33" s="37"/>
+      <c r="W33" s="37"/>
+      <c r="X33" s="37"/>
+      <c r="Y33" s="38"/>
+      <c r="Z33" s="19">
         <v>16</v>
       </c>
     </row>
@@ -2728,32 +2795,32 @@
       <c r="F34" s="16">
         <v>29</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="37"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U34" s="39"/>
-      <c r="V34" s="39"/>
-      <c r="W34" s="39"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="40"/>
-      <c r="Z34" s="43">
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U34" s="37"/>
+      <c r="V34" s="37"/>
+      <c r="W34" s="37"/>
+      <c r="X34" s="37"/>
+      <c r="Y34" s="38"/>
+      <c r="Z34" s="19">
         <v>17</v>
       </c>
     </row>
@@ -2764,30 +2831,32 @@
       <c r="F35" s="16">
         <v>30</v>
       </c>
-      <c r="G35" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="37"/>
-      <c r="Q35" s="37"/>
-      <c r="R35" s="37"/>
-      <c r="S35" s="37"/>
-      <c r="T35" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U35" s="39"/>
-      <c r="V35" s="39"/>
-      <c r="W35" s="39"/>
-      <c r="X35" s="39"/>
-      <c r="Y35" s="40"/>
-      <c r="Z35" s="43">
+      <c r="G35" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U35" s="37"/>
+      <c r="V35" s="37"/>
+      <c r="W35" s="37"/>
+      <c r="X35" s="37"/>
+      <c r="Y35" s="38"/>
+      <c r="Z35" s="19">
         <v>18</v>
       </c>
     </row>
@@ -2798,30 +2867,32 @@
       <c r="F36" s="16">
         <v>31</v>
       </c>
-      <c r="G36" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="37"/>
-      <c r="R36" s="37"/>
-      <c r="S36" s="37"/>
-      <c r="T36" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U36" s="41"/>
-      <c r="V36" s="41"/>
-      <c r="W36" s="41"/>
-      <c r="X36" s="41"/>
-      <c r="Y36" s="41"/>
-      <c r="AA36" s="43">
+      <c r="G36" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U36" s="39"/>
+      <c r="V36" s="39"/>
+      <c r="W36" s="39"/>
+      <c r="X36" s="39"/>
+      <c r="Y36" s="39"/>
+      <c r="AA36" s="19">
         <v>10</v>
       </c>
     </row>
@@ -2832,30 +2903,32 @@
       <c r="F37" s="16">
         <v>32</v>
       </c>
-      <c r="G37" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="37"/>
-      <c r="R37" s="37"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U37" s="39"/>
-      <c r="V37" s="39"/>
-      <c r="W37" s="39"/>
-      <c r="X37" s="39"/>
-      <c r="Y37" s="40"/>
-      <c r="Z37" s="43">
+      <c r="G37" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
+      <c r="W37" s="37"/>
+      <c r="X37" s="37"/>
+      <c r="Y37" s="38"/>
+      <c r="Z37" s="19">
         <v>19</v>
       </c>
     </row>
@@ -2866,30 +2939,32 @@
       <c r="F38" s="16">
         <v>33</v>
       </c>
-      <c r="G38" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="37"/>
-      <c r="R38" s="37"/>
-      <c r="S38" s="37"/>
-      <c r="T38" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="U38" s="41"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="41"/>
-      <c r="Y38" s="41"/>
-      <c r="AA38" s="43">
+      <c r="G38" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U38" s="39"/>
+      <c r="V38" s="39"/>
+      <c r="W38" s="39"/>
+      <c r="X38" s="39"/>
+      <c r="Y38" s="39"/>
+      <c r="AA38" s="19">
         <v>11</v>
       </c>
     </row>
@@ -2900,30 +2975,32 @@
       <c r="F39" s="16">
         <v>34</v>
       </c>
-      <c r="G39" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="37"/>
-      <c r="Q39" s="37"/>
-      <c r="R39" s="37"/>
-      <c r="S39" s="37"/>
-      <c r="T39" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U39" s="39"/>
-      <c r="V39" s="39"/>
-      <c r="W39" s="39"/>
-      <c r="X39" s="39"/>
-      <c r="Y39" s="40"/>
-      <c r="Z39" s="43">
+      <c r="G39" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U39" s="37"/>
+      <c r="V39" s="37"/>
+      <c r="W39" s="37"/>
+      <c r="X39" s="37"/>
+      <c r="Y39" s="38"/>
+      <c r="Z39" s="19">
         <v>20</v>
       </c>
     </row>
@@ -2931,14 +3008,14 @@
       <c r="F40" s="16">
         <v>35</v>
       </c>
-      <c r="G40" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="49"/>
+      <c r="G40" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="43"/>
       <c r="K40" s="44" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="L40" s="45"/>
       <c r="M40" s="45"/>
@@ -2948,15 +3025,15 @@
       <c r="Q40" s="45"/>
       <c r="R40" s="45"/>
       <c r="S40" s="46"/>
-      <c r="T40" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="52"/>
-      <c r="AA40" s="43">
+      <c r="T40" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="U40" s="48"/>
+      <c r="V40" s="48"/>
+      <c r="W40" s="48"/>
+      <c r="X40" s="48"/>
+      <c r="Y40" s="49"/>
+      <c r="AA40" s="19">
         <v>12</v>
       </c>
     </row>
@@ -2964,13 +3041,15 @@
       <c r="F41" s="16">
         <v>36</v>
       </c>
-      <c r="G41" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="44"/>
+      <c r="G41" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="44" t="s">
+        <v>176</v>
+      </c>
       <c r="L41" s="45"/>
       <c r="M41" s="45"/>
       <c r="N41" s="45"/>
@@ -2979,15 +3058,15 @@
       <c r="Q41" s="45"/>
       <c r="R41" s="45"/>
       <c r="S41" s="46"/>
-      <c r="T41" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U41" s="39"/>
-      <c r="V41" s="39"/>
-      <c r="W41" s="39"/>
-      <c r="X41" s="39"/>
-      <c r="Y41" s="40"/>
-      <c r="Z41" s="43">
+      <c r="T41" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U41" s="37"/>
+      <c r="V41" s="37"/>
+      <c r="W41" s="37"/>
+      <c r="X41" s="37"/>
+      <c r="Y41" s="38"/>
+      <c r="Z41" s="19">
         <v>21</v>
       </c>
     </row>
@@ -2995,13 +3074,15 @@
       <c r="F42" s="16">
         <v>37</v>
       </c>
-      <c r="G42" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="44"/>
+      <c r="G42" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="44" t="s">
+        <v>177</v>
+      </c>
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
       <c r="N42" s="45"/>
@@ -3010,15 +3091,15 @@
       <c r="Q42" s="45"/>
       <c r="R42" s="45"/>
       <c r="S42" s="46"/>
-      <c r="T42" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U42" s="39"/>
-      <c r="V42" s="39"/>
-      <c r="W42" s="39"/>
-      <c r="X42" s="39"/>
-      <c r="Y42" s="40"/>
-      <c r="Z42" s="43">
+      <c r="T42" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="U42" s="37"/>
+      <c r="V42" s="37"/>
+      <c r="W42" s="37"/>
+      <c r="X42" s="37"/>
+      <c r="Y42" s="38"/>
+      <c r="Z42" s="19">
         <v>22</v>
       </c>
     </row>
@@ -3026,13 +3107,15 @@
       <c r="F43" s="16">
         <v>38</v>
       </c>
-      <c r="G43" s="47" t="s">
-        <v>161</v>
-      </c>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="44"/>
+      <c r="G43" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="44" t="s">
+        <v>178</v>
+      </c>
       <c r="L43" s="45"/>
       <c r="M43" s="45"/>
       <c r="N43" s="45"/>
@@ -3041,15 +3124,15 @@
       <c r="Q43" s="45"/>
       <c r="R43" s="45"/>
       <c r="S43" s="46"/>
-      <c r="T43" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="U43" s="51"/>
-      <c r="V43" s="51"/>
-      <c r="W43" s="51"/>
-      <c r="X43" s="51"/>
-      <c r="Y43" s="52"/>
-      <c r="AA43" s="43">
+      <c r="T43" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="U43" s="48"/>
+      <c r="V43" s="48"/>
+      <c r="W43" s="48"/>
+      <c r="X43" s="48"/>
+      <c r="Y43" s="49"/>
+      <c r="AA43" s="19">
         <v>13</v>
       </c>
     </row>
@@ -3057,13 +3140,15 @@
       <c r="F44" s="16">
         <v>39</v>
       </c>
-      <c r="G44" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="44"/>
+      <c r="G44" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="44" t="s">
+        <v>179</v>
+      </c>
       <c r="L44" s="45"/>
       <c r="M44" s="45"/>
       <c r="N44" s="45"/>
@@ -3072,15 +3157,15 @@
       <c r="Q44" s="45"/>
       <c r="R44" s="45"/>
       <c r="S44" s="46"/>
-      <c r="T44" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="U44" s="51"/>
-      <c r="V44" s="51"/>
-      <c r="W44" s="51"/>
-      <c r="X44" s="51"/>
-      <c r="Y44" s="52"/>
-      <c r="AA44" s="43">
+      <c r="T44" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="U44" s="48"/>
+      <c r="V44" s="48"/>
+      <c r="W44" s="48"/>
+      <c r="X44" s="48"/>
+      <c r="Y44" s="49"/>
+      <c r="AA44" s="19">
         <v>14</v>
       </c>
     </row>
@@ -3128,6 +3213,12 @@
     <mergeCell ref="T20:Y20"/>
     <mergeCell ref="T21:Y21"/>
     <mergeCell ref="T34:Y34"/>
+    <mergeCell ref="T23:Y23"/>
+    <mergeCell ref="T25:Y25"/>
+    <mergeCell ref="T26:Y26"/>
+    <mergeCell ref="T27:Y27"/>
+    <mergeCell ref="T28:Y28"/>
+    <mergeCell ref="T22:Y22"/>
     <mergeCell ref="T35:Y35"/>
     <mergeCell ref="T36:Y36"/>
     <mergeCell ref="T37:Y37"/>
@@ -3137,12 +3228,6 @@
     <mergeCell ref="T31:Y31"/>
     <mergeCell ref="T32:Y32"/>
     <mergeCell ref="T33:Y33"/>
-    <mergeCell ref="T23:Y23"/>
-    <mergeCell ref="T25:Y25"/>
-    <mergeCell ref="T26:Y26"/>
-    <mergeCell ref="T27:Y27"/>
-    <mergeCell ref="T28:Y28"/>
-    <mergeCell ref="T22:Y22"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="K4:S4"/>
@@ -3200,6 +3285,10 @@
     <mergeCell ref="K31:S31"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="K32:S32"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="K38:S38"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="K39:S39"/>
     <mergeCell ref="G33:J33"/>
     <mergeCell ref="K33:S33"/>
     <mergeCell ref="G34:J34"/>
@@ -3210,10 +3299,6 @@
     <mergeCell ref="K36:S36"/>
     <mergeCell ref="G37:J37"/>
     <mergeCell ref="K37:S37"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="K38:S38"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="K39:S39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4465,7 +4550,7 @@
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
@@ -4869,7 +4954,7 @@
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -5165,7 +5250,7 @@
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
       <c r="X28" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y28" s="11"/>
       <c r="Z28" s="11"/>
@@ -6049,7 +6134,7 @@
       <c r="V38" s="11"/>
       <c r="W38" s="11"/>
       <c r="X38" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y38" s="11"/>
       <c r="Z38" s="11"/>
@@ -6655,11 +6740,11 @@
       <c r="F49" s="10">
         <v>1</v>
       </c>
-      <c r="G49" s="24" t="s">
+      <c r="G49" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
@@ -6709,11 +6794,11 @@
       <c r="F50" s="10">
         <v>2</v>
       </c>
-      <c r="G50" s="24" t="s">
+      <c r="G50" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11" t="s">
         <v>54</v>
@@ -6765,11 +6850,11 @@
       <c r="F51" s="10">
         <v>3</v>
       </c>
-      <c r="G51" s="24" t="s">
+      <c r="G51" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11" t="s">
         <v>55</v>
@@ -6821,11 +6906,11 @@
       <c r="F52" s="10">
         <v>4</v>
       </c>
-      <c r="G52" s="24" t="s">
+      <c r="G52" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11" t="s">
         <v>56</v>
@@ -6877,11 +6962,11 @@
       <c r="F53" s="10">
         <v>5</v>
       </c>
-      <c r="G53" s="24" t="s">
+      <c r="G53" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
@@ -6931,11 +7016,11 @@
       <c r="F54" s="10">
         <v>6</v>
       </c>
-      <c r="G54" s="24" t="s">
+      <c r="G54" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="50"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
       <c r="L54" s="11"/>
@@ -6985,11 +7070,11 @@
       <c r="F55" s="10">
         <v>7</v>
       </c>
-      <c r="G55" s="24" t="s">
+      <c r="G55" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="50"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
       <c r="L55" s="11"/>
@@ -7033,11 +7118,11 @@
       <c r="F56" s="10">
         <v>8</v>
       </c>
-      <c r="G56" s="24" t="s">
+      <c r="G56" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="50"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
       <c r="L56" s="11"/>
@@ -7081,11 +7166,11 @@
       <c r="F57" s="10">
         <v>9</v>
       </c>
-      <c r="G57" s="24" t="s">
+      <c r="G57" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="50"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
@@ -7129,11 +7214,11 @@
       <c r="F58" s="10">
         <v>10</v>
       </c>
-      <c r="G58" s="24" t="s">
+      <c r="G58" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="50"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
       <c r="L58" s="11"/>
@@ -7862,15 +7947,15 @@
       <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="11">
         <v>1</v>
       </c>
@@ -7880,15 +7965,15 @@
       <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26" t="s">
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="11">
         <v>2</v>
       </c>
@@ -7898,15 +7983,15 @@
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26" t="s">
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="11">
         <v>3</v>
       </c>
@@ -7916,15 +8001,15 @@
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26" t="s">
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="11">
         <v>3</v>
       </c>
@@ -7934,15 +8019,15 @@
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26" t="s">
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="52"/>
       <c r="H8" s="11">
         <v>4</v>
       </c>
@@ -7952,15 +8037,15 @@
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="11">
         <v>5</v>
       </c>
@@ -7970,15 +8055,15 @@
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="11">
         <v>6</v>
       </c>
@@ -7988,15 +8073,15 @@
       <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26" t="s">
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="11">
         <v>4</v>
       </c>
@@ -8006,15 +8091,15 @@
       <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26" t="s">
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="52"/>
       <c r="H12" s="11">
         <v>5</v>
       </c>
@@ -8024,15 +8109,15 @@
       <c r="B13" s="9">
         <v>10</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26" t="s">
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="26"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="11">
         <v>3</v>
       </c>
@@ -8042,15 +8127,15 @@
       <c r="B14" s="9">
         <v>11</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26" t="s">
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="26"/>
+      <c r="G14" s="52"/>
       <c r="H14" s="11">
         <v>5</v>
       </c>
@@ -8060,9 +8145,9 @@
       <c r="B15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>

</xml_diff>